<commit_message>
Fixed bugs in the code
Changed data files and linked each category to appropriate data set
</commit_message>
<xml_diff>
--- a/data/ACS_5YR_DP05_metadata.xlsx
+++ b/data/ACS_5YR_DP05_metadata.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddudussa/OneDrive - Georgia Institute of Technology/GitHub/adussa3.github.io/projects/AtlantaPopulationEstimate/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddudussa/Downloads/ACS_16_5YR_DP05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0763076-CDD6-F94D-9500-FCCFA750997F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C70657FF-9685-A14A-A19D-BE9B47D781A3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
-    <sheet name="ACS_5YR_DP05_metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="ACS_16_5YR_DP05_metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="168" uniqueCount="160">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="174" uniqueCount="172">
   <si>
     <t>GEO.id</t>
   </si>
@@ -59,457 +54,493 @@
     <t>HC01_VC04</t>
   </si>
   <si>
-    <t>Estimate; SEX AND AGE - Male</t>
+    <t>Estimate; SEX AND AGE - Total population - Male</t>
   </si>
   <si>
     <t>HC01_VC05</t>
   </si>
   <si>
-    <t>Estimate; SEX AND AGE - Female</t>
-  </si>
-  <si>
-    <t>HC01_VC07</t>
+    <t>Estimate; SEX AND AGE - Total population - Female</t>
+  </si>
+  <si>
+    <t>HC01_VC08</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - Under 5 years</t>
   </si>
   <si>
-    <t>HC01_VC08</t>
+    <t>HC01_VC09</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 5 to 9 years</t>
   </si>
   <si>
-    <t>HC01_VC09</t>
+    <t>HC01_VC10</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 10 to 14 years</t>
   </si>
   <si>
-    <t>HC01_VC10</t>
+    <t>HC01_VC11</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 15 to 19 years</t>
   </si>
   <si>
-    <t>HC01_VC11</t>
+    <t>HC01_VC12</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 20 to 24 years</t>
   </si>
   <si>
-    <t>HC01_VC12</t>
+    <t>HC01_VC13</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 25 to 34 years</t>
   </si>
   <si>
-    <t>HC01_VC13</t>
+    <t>HC01_VC14</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 35 to 44 years</t>
   </si>
   <si>
-    <t>HC01_VC14</t>
+    <t>HC01_VC15</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 45 to 54 years</t>
   </si>
   <si>
-    <t>HC01_VC15</t>
+    <t>HC01_VC16</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 55 to 59 years</t>
   </si>
   <si>
-    <t>HC01_VC16</t>
+    <t>HC01_VC17</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 60 to 64 years</t>
   </si>
   <si>
-    <t>HC01_VC17</t>
+    <t>HC01_VC18</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 65 to 74 years</t>
   </si>
   <si>
-    <t>HC01_VC18</t>
+    <t>HC01_VC19</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 75 to 84 years</t>
   </si>
   <si>
-    <t>HC01_VC19</t>
+    <t>HC01_VC20</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 85 years and over</t>
   </si>
   <si>
-    <t>HC01_VC21</t>
+    <t>HC01_VC23</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - Median age (years)</t>
   </si>
   <si>
-    <t>HC01_VC23</t>
+    <t>HC01_VC26</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 18 years and over</t>
   </si>
   <si>
-    <t>HC01_VC24</t>
+    <t>HC01_VC27</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 21 years and over</t>
   </si>
   <si>
-    <t>HC01_VC25</t>
+    <t>HC01_VC28</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 62 years and over</t>
   </si>
   <si>
-    <t>HC01_VC26</t>
+    <t>HC01_VC29</t>
   </si>
   <si>
     <t>Estimate; SEX AND AGE - 65 years and over</t>
   </si>
   <si>
-    <t>HC01_VC28</t>
-  </si>
-  <si>
-    <t>HC01_VC29</t>
-  </si>
-  <si>
-    <t>HC01_VC30</t>
-  </si>
-  <si>
     <t>HC01_VC32</t>
   </si>
   <si>
     <t>HC01_VC33</t>
   </si>
   <si>
+    <t>Estimate; SEX AND AGE - 18 years and over - Male</t>
+  </si>
+  <si>
     <t>HC01_VC34</t>
   </si>
   <si>
+    <t>Estimate; SEX AND AGE - 18 years and over - Female</t>
+  </si>
+  <si>
+    <t>HC01_VC37</t>
+  </si>
+  <si>
     <t>HC01_VC38</t>
   </si>
   <si>
+    <t>Estimate; SEX AND AGE - 65 years and over - Male</t>
+  </si>
+  <si>
+    <t>HC01_VC39</t>
+  </si>
+  <si>
+    <t>Estimate; SEX AND AGE - 65 years and over - Female</t>
+  </si>
+  <si>
+    <t>HC01_VC43</t>
+  </si>
+  <si>
     <t>Estimate; RACE - Total population</t>
   </si>
   <si>
-    <t>HC01_VC39</t>
+    <t>HC01_VC44</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Total population - One race</t>
+  </si>
+  <si>
+    <t>HC01_VC45</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Total population - Two or more races</t>
+  </si>
+  <si>
+    <t>HC01_VC48</t>
   </si>
   <si>
     <t>Estimate; RACE - One race</t>
   </si>
   <si>
-    <t>HC01_VC40</t>
+    <t>HC01_VC49</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - White</t>
+  </si>
+  <si>
+    <t>HC01_VC50</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Black or African American</t>
+  </si>
+  <si>
+    <t>HC01_VC51</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - American Indian and Alaska Native</t>
+  </si>
+  <si>
+    <t>HC01_VC52</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - American Indian and Alaska Native - Cherokee tribal grouping</t>
+  </si>
+  <si>
+    <t>HC01_VC53</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - American Indian and Alaska Native - Chippewa tribal grouping</t>
+  </si>
+  <si>
+    <t>HC01_VC54</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - American Indian and Alaska Native - Navajo tribal grouping</t>
+  </si>
+  <si>
+    <t>HC01_VC55</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - American Indian and Alaska Native - Sioux tribal grouping</t>
+  </si>
+  <si>
+    <t>HC01_VC56</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian</t>
+  </si>
+  <si>
+    <t>HC01_VC57</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Asian Indian</t>
+  </si>
+  <si>
+    <t>HC01_VC58</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Chinese</t>
+  </si>
+  <si>
+    <t>HC01_VC59</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Filipino</t>
+  </si>
+  <si>
+    <t>HC01_VC60</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Japanese</t>
+  </si>
+  <si>
+    <t>HC01_VC61</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Korean</t>
+  </si>
+  <si>
+    <t>HC01_VC62</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Vietnamese</t>
+  </si>
+  <si>
+    <t>HC01_VC63</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Asian - Other Asian</t>
+  </si>
+  <si>
+    <t>HC01_VC64</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>HC01_VC65</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Native Hawaiian</t>
+  </si>
+  <si>
+    <t>HC01_VC66</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Guamanian or Chamorro</t>
+  </si>
+  <si>
+    <t>HC01_VC67</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Samoan</t>
+  </si>
+  <si>
+    <t>HC01_VC68</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>HC01_VC69</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - One race - Some other race</t>
+  </si>
+  <si>
+    <t>HC01_VC70</t>
   </si>
   <si>
     <t>Estimate; RACE - Two or more races</t>
   </si>
   <si>
-    <t>HC01_VC42</t>
-  </si>
-  <si>
-    <t>HC01_VC43</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - White</t>
-  </si>
-  <si>
-    <t>HC01_VC44</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Black or African American</t>
-  </si>
-  <si>
-    <t>HC01_VC45</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - American Indian and Alaska Native</t>
-  </si>
-  <si>
-    <t>HC01_VC46</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - American Indian and Alaska Native - Cherokee tribal grouping</t>
-  </si>
-  <si>
-    <t>HC01_VC47</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - American Indian and Alaska Native - Chippewa tribal grouping</t>
-  </si>
-  <si>
-    <t>HC01_VC48</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - American Indian and Alaska Native - Navajo tribal grouping</t>
-  </si>
-  <si>
-    <t>HC01_VC49</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - American Indian and Alaska Native - Sioux tribal grouping</t>
-  </si>
-  <si>
-    <t>HC01_VC50</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian</t>
-  </si>
-  <si>
-    <t>HC01_VC51</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Asian Indian</t>
-  </si>
-  <si>
-    <t>HC01_VC52</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Chinese</t>
-  </si>
-  <si>
-    <t>HC01_VC53</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Filipino</t>
-  </si>
-  <si>
-    <t>HC01_VC54</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Japanese</t>
-  </si>
-  <si>
-    <t>HC01_VC55</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Korean</t>
-  </si>
-  <si>
-    <t>HC01_VC56</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Vietnamese</t>
-  </si>
-  <si>
-    <t>HC01_VC57</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Asian - Other Asian</t>
-  </si>
-  <si>
-    <t>HC01_VC58</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander</t>
-  </si>
-  <si>
-    <t>HC01_VC59</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Native Hawaiian</t>
-  </si>
-  <si>
-    <t>HC01_VC60</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Guamanian or Chamorro</t>
-  </si>
-  <si>
-    <t>HC01_VC61</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Samoan</t>
-  </si>
-  <si>
-    <t>HC01_VC62</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Native Hawaiian and Other Pacific Islander - Other Pacific Islander</t>
-  </si>
-  <si>
-    <t>HC01_VC63</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - One race - Some other race</t>
-  </si>
-  <si>
-    <t>HC01_VC64</t>
-  </si>
-  <si>
-    <t>HC01_VC65</t>
+    <t>HC01_VC71</t>
   </si>
   <si>
     <t>Estimate; RACE - Two or more races - White and Black or African American</t>
   </si>
   <si>
-    <t>HC01_VC66</t>
+    <t>HC01_VC72</t>
   </si>
   <si>
     <t>Estimate; RACE - Two or more races - White and American Indian and Alaska Native</t>
   </si>
   <si>
-    <t>HC01_VC67</t>
+    <t>HC01_VC73</t>
   </si>
   <si>
     <t>Estimate; RACE - Two or more races - White and Asian</t>
   </si>
   <si>
-    <t>HC01_VC68</t>
+    <t>HC01_VC74</t>
   </si>
   <si>
     <t>Estimate; RACE - Two or more races - Black or African American and American Indian and Alaska Native</t>
   </si>
   <si>
-    <t>HC01_VC71</t>
+    <t>HC01_VC77</t>
   </si>
   <si>
     <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population</t>
   </si>
   <si>
-    <t>HC01_VC72</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - White</t>
-  </si>
-  <si>
-    <t>HC01_VC73</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - Black or African American</t>
-  </si>
-  <si>
-    <t>HC01_VC74</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - American Indian and Alaska Native</t>
-  </si>
-  <si>
-    <t>HC01_VC75</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - Asian</t>
-  </si>
-  <si>
-    <t>HC01_VC76</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - Native Hawaiian and Other Pacific Islander</t>
-  </si>
-  <si>
-    <t>HC01_VC77</t>
-  </si>
-  <si>
-    <t>Estimate; RACE - Some other race</t>
+    <t>HC01_VC78</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - White</t>
+  </si>
+  <si>
+    <t>HC01_VC79</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - Black or African American</t>
+  </si>
+  <si>
+    <t>HC01_VC80</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - American Indian and Alaska Native</t>
   </si>
   <si>
     <t>HC01_VC81</t>
   </si>
   <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - Asian</t>
+  </si>
+  <si>
+    <t>HC01_VC82</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - Native Hawaiian and Other Pacific Islander</t>
+  </si>
+  <si>
+    <t>HC01_VC83</t>
+  </si>
+  <si>
+    <t>Estimate; RACE - Race alone or in combination with one or more other races - Total population - Some other race</t>
+  </si>
+  <si>
+    <t>HC01_VC87</t>
+  </si>
+  <si>
     <t>Estimate; HISPANIC OR LATINO AND RACE - Total population</t>
   </si>
   <si>
-    <t>HC01_VC82</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Hispanic or Latino (of any race)</t>
-  </si>
-  <si>
-    <t>HC01_VC83</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Hispanic or Latino (of any race) - Mexican</t>
-  </si>
-  <si>
-    <t>HC01_VC84</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Hispanic or Latino (of any race) - Puerto Rican</t>
-  </si>
-  <si>
-    <t>HC01_VC85</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Hispanic or Latino (of any race) - Cuban</t>
-  </si>
-  <si>
-    <t>HC01_VC86</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Hispanic or Latino (of any race) - Other Hispanic or Latino</t>
-  </si>
-  <si>
-    <t>HC01_VC87</t>
-  </si>
-  <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino</t>
-  </si>
-  <si>
     <t>HC01_VC88</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - White alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Hispanic or Latino (of any race)</t>
   </si>
   <si>
     <t>HC01_VC89</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Black or African American alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Hispanic or Latino (of any race) - Mexican</t>
   </si>
   <si>
     <t>HC01_VC90</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - American Indian and Alaska Native alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Hispanic or Latino (of any race) - Puerto Rican</t>
   </si>
   <si>
     <t>HC01_VC91</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Asian alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Hispanic or Latino (of any race) - Cuban</t>
   </si>
   <si>
     <t>HC01_VC92</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Native Hawaiian and Other Pacific Islander alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Hispanic or Latino (of any race) - Other Hispanic or Latino</t>
   </si>
   <si>
     <t>HC01_VC93</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Some other race alone</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino</t>
   </si>
   <si>
     <t>HC01_VC94</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Two or more races</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - White alone</t>
   </si>
   <si>
     <t>HC01_VC95</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Two or more races - Two races including Some other race</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Black or African American alone</t>
   </si>
   <si>
     <t>HC01_VC96</t>
   </si>
   <si>
-    <t>Estimate; HISPANIC OR LATINO AND RACE - Not Hispanic or Latino - Two or more races - Two races excluding Some other race, and Three or more races</t>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - American Indian and Alaska Native alone</t>
+  </si>
+  <si>
+    <t>HC01_VC97</t>
+  </si>
+  <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Asian alone</t>
   </si>
   <si>
     <t>HC01_VC98</t>
   </si>
   <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Native Hawaiian and Other Pacific Islander alone</t>
+  </si>
+  <si>
+    <t>HC01_VC99</t>
+  </si>
+  <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Some other race alone</t>
+  </si>
+  <si>
+    <t>HC01_VC100</t>
+  </si>
+  <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Two or more races</t>
+  </si>
+  <si>
+    <t>HC01_VC101</t>
+  </si>
+  <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Two or more races - Two races including Some other race</t>
+  </si>
+  <si>
+    <t>HC01_VC102</t>
+  </si>
+  <si>
+    <t>Estimate; HISPANIC OR LATINO AND RACE - Total population - Not Hispanic or Latino - Two or more races - Two races excluding Some other race, and Three or more races</t>
+  </si>
+  <si>
+    <t>HC01_VC104</t>
+  </si>
+  <si>
     <t>Estimate; HISPANIC OR LATINO AND RACE - Total housing units</t>
+  </si>
+  <si>
+    <t>HC01_VC108</t>
+  </si>
+  <si>
+    <t>Estimate; CITIZEN, VOTING AGE POPULATION - Citizen, 18 and over population</t>
+  </si>
+  <si>
+    <t>HC01_VC109</t>
+  </si>
+  <si>
+    <t>Estimate; CITIZEN, VOTING AGE POPULATION - Citizen, 18 and over population - Male</t>
+  </si>
+  <si>
+    <t>HC01_VC110</t>
+  </si>
+  <si>
+    <t>Estimate; CITIZEN, VOTING AGE POPULATION - Citizen, 18 and over population - Female</t>
   </si>
 </sst>
 </file>
@@ -1350,13 +1381,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B324"/>
+  <dimension ref="A1:B336"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B325" activeCellId="12" sqref="A277:B279 A281:B283 A285:B287 A289:B291 A293:B295 A297:B299 A301:B303 A305:B307 A309:B311 A313:B315 A317:B319 A321:B323 A325:B327"/>
+    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
+      <selection activeCell="B339" sqref="B339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="157.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1563,20 +1598,20 @@
         <v>49</v>
       </c>
       <c r="B92" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B100" t="s">
         <v>47</v>
@@ -1584,450 +1619,474 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B108" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B112" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B116" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B120" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="B124" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B128" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B132" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B136" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B140" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B144" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B148" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B152" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B156" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B160" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B164" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B168" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B172" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B176" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
     </row>
     <row r="180" spans="1:2">
       <c r="A180" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B180" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B184" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B188" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B192" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B196" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B200" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="204" spans="1:2">
       <c r="A204" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B204" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B208" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B212" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="B216" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
     </row>
     <row r="220" spans="1:2">
       <c r="A220" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B220" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="224" spans="1:2">
       <c r="A224" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B224" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B228" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B232" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B236" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B240" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B244" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B248" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B252" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="B256" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="260" spans="1:2">
       <c r="A260" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B260" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="264" spans="1:2">
       <c r="A264" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="B264" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="268" spans="1:2">
       <c r="A268" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B268" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
     </row>
     <row r="272" spans="1:2">
       <c r="A272" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="B272" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="276" spans="1:2">
       <c r="A276" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="B276" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="280" spans="1:2">
       <c r="A280" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="B280" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
     </row>
     <row r="284" spans="1:2">
       <c r="A284" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B284" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="288" spans="1:2">
       <c r="A288" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B288" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="292" spans="1:2">
       <c r="A292" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B292" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
     </row>
     <row r="296" spans="1:2">
       <c r="A296" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B296" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
     </row>
     <row r="300" spans="1:2">
       <c r="A300" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B300" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="304" spans="1:2">
       <c r="A304" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="B304" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
     </row>
     <row r="308" spans="1:2">
       <c r="A308" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="B308" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
     </row>
     <row r="312" spans="1:2">
       <c r="A312" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="B312" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="316" spans="1:2">
       <c r="A316" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B316" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
     </row>
     <row r="320" spans="1:2">
       <c r="A320" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="B320" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
     </row>
     <row r="324" spans="1:2">
       <c r="A324" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="B324" t="s">
-        <v>159</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" t="s">
+        <v>166</v>
+      </c>
+      <c r="B328" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>168</v>
+      </c>
+      <c r="B332" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>170</v>
+      </c>
+      <c r="B336" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>